<commit_message>
Aug 10:Naidu:Merged with Sudheers changes
</commit_message>
<xml_diff>
--- a/src/test/java/resources/TestData/ActiTimeData.xlsx
+++ b/src/test/java/resources/TestData/ActiTimeData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>custName</t>
   </si>
@@ -36,28 +36,13 @@
     <t>I work in Techm</t>
   </si>
   <si>
-    <t>TC002</t>
-  </si>
-  <si>
     <t>TcName</t>
   </si>
   <si>
-    <t>TC003</t>
-  </si>
-  <si>
-    <t>TC005</t>
-  </si>
-  <si>
-    <t>TC006</t>
-  </si>
-  <si>
-    <t>TC008</t>
-  </si>
-  <si>
-    <t>Ruthwik</t>
-  </si>
-  <si>
     <t>TC001_CreateCustomer</t>
+  </si>
+  <si>
+    <t>TC002_deleteCustomer</t>
   </si>
 </sst>
 </file>
@@ -398,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -413,7 +398,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -424,7 +409,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -435,7 +420,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -457,56 +442,12 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>